<commit_message>
block 3 drawing still incomplete
</commit_message>
<xml_diff>
--- a/ofc/2081_82 yojana haru.xlsx
+++ b/ofc/2081_82 yojana haru.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -270,12 +270,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -290,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -300,13 +312,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -613,15 +631,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="68.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -691,13 +709,13 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="11">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="14">
         <v>250000</v>
       </c>
     </row>
@@ -713,134 +731,134 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="11">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="14">
         <v>200000</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="11">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="14">
         <v>200000</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="14">
         <v>200000</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12" s="11">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="14">
         <v>300000</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="11">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="14">
         <v>200000</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="11">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="14">
         <v>200000</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="11">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="14">
         <v>300000</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="11">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="14">
         <v>300000</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17" s="11">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="14">
         <v>100000</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18" s="11">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="14">
         <v>100000</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19" s="11">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="14">
         <v>200000</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20" s="11">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="14">
         <v>1000000</v>
       </c>
     </row>
@@ -884,68 +902,68 @@
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25" s="11">
         <v>21</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="14">
         <v>500000</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26" s="11">
         <v>22</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="14">
         <v>400000</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27" s="11">
         <v>23</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="11">
         <v>1600000</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28" s="11">
         <v>24</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="14">
         <v>400000</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="A29" s="11">
         <v>25</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="14">
         <v>300000</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="A30" s="11">
         <v>26</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="14">
         <v>500000</v>
       </c>
     </row>
@@ -964,24 +982,24 @@
       <c r="C32" s="1"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="A33" s="11">
         <v>27</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="14">
         <v>200000</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="A34" s="11">
         <v>28</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34" s="14">
         <v>1000000</v>
       </c>
     </row>
@@ -993,13 +1011,13 @@
       <c r="C35" s="1"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+      <c r="A36" s="11">
         <v>29</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="14">
         <v>500000</v>
       </c>
     </row>
@@ -1018,68 +1036,68 @@
       <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+      <c r="A39" s="11">
         <v>30</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39" s="11">
         <v>1600000</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+      <c r="A40" s="11">
         <v>31</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40" s="14">
         <v>500000</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+      <c r="A41" s="11">
         <v>32</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" s="11">
         <v>1600000</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+      <c r="A42" s="11">
         <v>33</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="11">
         <v>5000000</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+      <c r="A43" s="11">
         <v>34</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="11">
         <v>2500000</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+      <c r="A44" s="15">
         <v>35</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="8">
+      <c r="C44" s="17">
         <v>2100000</v>
       </c>
     </row>
@@ -1090,13 +1108,13 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+      <c r="A46" s="11">
         <v>36</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="14">
         <v>500000</v>
       </c>
     </row>
@@ -1107,42 +1125,43 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
+      <c r="A48" s="11">
         <v>36</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48" s="14">
         <v>400000</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="6" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="10"/>
+      <c r="B49" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C49" s="11">
         <v>1600000</v>
       </c>
-      <c r="D49" s="1">
+      <c r="D49" s="3">
         <f>SUM(C25:C49)-C44</f>
         <v>19100000</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" s="6" t="s">
         <v>53</v>
       </c>
@@ -1150,35 +1169,35 @@
         <v>1304700</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="9" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="10" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="8" t="s">
         <v>55</v>
       </c>
       <c r="C56" s="1">
         <v>2660000</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="9" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="10" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C58" s="1">
         <v>10000000</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C60" s="11">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C60" s="9">
         <f>SUM(C2:C58)</f>
         <v>40164700</v>
       </c>

</xml_diff>

<commit_message>
nmbering in yojana 2081-2082
</commit_message>
<xml_diff>
--- a/ofc/2081_82 yojana haru.xlsx
+++ b/ofc/2081_82 yojana haru.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$58</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
@@ -631,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,7 +1129,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B48" s="13" t="s">
         <v>49</v>
@@ -1136,7 +1139,9 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="10"/>
+      <c r="A49" s="11">
+        <v>38</v>
+      </c>
       <c r="B49" s="13" t="s">
         <v>50</v>
       </c>
@@ -1162,6 +1167,9 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>39</v>
+      </c>
       <c r="B53" s="6" t="s">
         <v>53</v>
       </c>
@@ -1175,6 +1183,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>40</v>
+      </c>
       <c r="B56" s="8" t="s">
         <v>55</v>
       </c>
@@ -1189,6 +1200,9 @@
       <c r="C57" s="1"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>41</v>
+      </c>
       <c r="B58" s="8" t="s">
         <v>57</v>
       </c>
@@ -1204,6 +1218,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="85" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
kurthali sadak estimate given, new tahara naksha at nagar hospital muni rajkulo near, chinimaya mam bora estimate, setidevi mandir valuation complete
</commit_message>
<xml_diff>
--- a/ofc/2081_82 yojana haru.xlsx
+++ b/ofc/2081_82 yojana haru.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$58</definedName>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
   <si>
     <t>क्र. सं</t>
   </si>
@@ -207,6 +208,69 @@
   </si>
   <si>
     <t xml:space="preserve">खुलालटार सानागाउँ उखुटार सडक शंखरापुर ९ </t>
+  </si>
+  <si>
+    <t>S.No.</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Interlocking block</t>
+  </si>
+  <si>
+    <t>Sqm</t>
+  </si>
+  <si>
+    <t>Stone soling</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>RCC road</t>
+  </si>
+  <si>
+    <t>Km</t>
+  </si>
+  <si>
+    <t>Hume pipe</t>
+  </si>
+  <si>
+    <t>no.</t>
+  </si>
+  <si>
+    <t>Mandir</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Drain sarsafai</t>
+  </si>
+  <si>
+    <t>Sarbajanik bhawan</t>
+  </si>
+  <si>
+    <t>Sarbajanik Dhaara nirmaan</t>
+  </si>
+  <si>
+    <t>paati nirmaan</t>
+  </si>
+  <si>
+    <t>Ward 9</t>
+  </si>
+  <si>
+    <t>Mangaal</t>
   </si>
 </sst>
 </file>
@@ -293,7 +357,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -301,11 +365,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -328,6 +407,10 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,7 +717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A16" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:C58"/>
     </sheetView>
   </sheetViews>
@@ -1220,4 +1303,202 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="85" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="H8:L19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H9" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H10" s="19">
+        <v>1</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="K10" s="18">
+        <v>135</v>
+      </c>
+      <c r="L10" s="18"/>
+    </row>
+    <row r="11" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H11" s="19">
+        <v>2</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="K11" s="18">
+        <f>11.85</f>
+        <v>11.85</v>
+      </c>
+      <c r="L11" s="18"/>
+    </row>
+    <row r="12" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H12" s="19">
+        <v>3</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="K12" s="18">
+        <f>(20.2+13.8)/1000</f>
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="L12" s="18"/>
+    </row>
+    <row r="13" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H13" s="19">
+        <v>4</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="K13" s="18">
+        <v>1</v>
+      </c>
+      <c r="L13" s="18"/>
+    </row>
+    <row r="14" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H14" s="19">
+        <v>5</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="K14" s="18">
+        <v>65</v>
+      </c>
+      <c r="L14" s="18"/>
+    </row>
+    <row r="15" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H15" s="19">
+        <v>6</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="K15" s="18">
+        <v>1</v>
+      </c>
+      <c r="L15" s="18"/>
+    </row>
+    <row r="16" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H16" s="19">
+        <v>7</v>
+      </c>
+      <c r="I16" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="J16" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="K16" s="18">
+        <v>112.3</v>
+      </c>
+      <c r="L16" s="18"/>
+    </row>
+    <row r="17" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H17" s="19">
+        <v>8</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="K17" s="18">
+        <v>2</v>
+      </c>
+      <c r="L17" s="18"/>
+    </row>
+    <row r="18" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H18" s="19">
+        <v>9</v>
+      </c>
+      <c r="I18" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="J18" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="K18" s="18">
+        <v>1</v>
+      </c>
+      <c r="L18" s="18"/>
+    </row>
+    <row r="19" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H19" s="20">
+        <v>10</v>
+      </c>
+      <c r="I19" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="J19" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="K19" s="21">
+        <v>2</v>
+      </c>
+      <c r="L19" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
complete tahara and report to prakash sir
</commit_message>
<xml_diff>
--- a/ofc/2081_82 yojana haru.xlsx
+++ b/ofc/2081_82 yojana haru.xlsx
@@ -12,6 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$58</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$G$7:$M$20</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -1310,7 +1311,7 @@
   <dimension ref="H8:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="G7" sqref="G7:M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1324,7 +1325,7 @@
   </cols>
   <sheetData>
     <row r="8" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H8" t="s">
+      <c r="H8" s="4" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1499,6 +1500,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LPrepared By:
+Kristal Suwal&amp;RApproved By:
+Er. Prakash Singh Saud</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
बिनोदtahara complete and sadak details added
</commit_message>
<xml_diff>
--- a/ofc/2081_82 yojana haru.xlsx
+++ b/ofc/2081_82 yojana haru.xlsx
@@ -4,22 +4,153 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Baato" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$58</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$G$7:$M$20</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="E20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+नेपाल सरकार को मापदण्ड बमोजिम</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D21" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+सुप्रिम अदालत </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E21" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+नेपाल सरकार को मापदण्ड बमोजिम</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D23" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+सुप्रिम अदालत </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D25" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+नेपाल सरकार को मापदण्ड बमोजिम</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="126">
   <si>
     <t>क्र. सं</t>
   </si>
@@ -273,15 +404,156 @@
   <si>
     <t>Mangaal</t>
   </si>
+  <si>
+    <t>क्र. सं.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">सडकको नाम/किसिम </t>
+  </si>
+  <si>
+    <t xml:space="preserve">लम्बाई </t>
+  </si>
+  <si>
+    <t xml:space="preserve">चौदाई </t>
+  </si>
+  <si>
+    <t xml:space="preserve">कैफियत </t>
+  </si>
+  <si>
+    <t xml:space="preserve">कागेस्वोरी चक्रपथ सडक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">सानागाउँ टोल भित्रि सडक </t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">मगर टोल कुर्थली सडक </t>
+  </si>
+  <si>
+    <t>इन्द्रायणी चनौटे भेटेनरी उखुटार लकिल्ला सडक</t>
+  </si>
+  <si>
+    <t xml:space="preserve">पासिखेल नया हे.पो.राज कुलो सडक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">गैराघर ढुन्दोल धर्मपाल उखुटार सडक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">भेटेनरी सुवेल गाउँ पन्चकन्या चनौटे सडक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">साना गाउँ उखुटार सडक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">लकिल्ला भुमेथली सडक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">इन्द्रायणी पुखुलाछी सडक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">लकिल्ला घट्टेखोला गागल सडक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">इन्द्रायणी मन्दिर मनमत्ता सडक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">का. च. देवि स्थान भुमैटार सडक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">भुमेथली राजकुलो हुँदै रामप्रसाद घर बाटो </t>
+  </si>
+  <si>
+    <t xml:space="preserve">पासिखेल सानागाउँ जाने चोकदेखि रा. उ. मा. वि. जोड्ने सडक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">भेटेनरी बाहुन डाँडा सडक पताली </t>
+  </si>
+  <si>
+    <t xml:space="preserve">साँखु चक्रपथ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">खहरे खोला/ राजकुलो भएकोमा दायाँ बायाँ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">मनोहरा खोला दायाँ बायाँ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">सहायक खोला </t>
+  </si>
+  <si>
+    <t xml:space="preserve">महादेव खोला, गडगडे खोला, नाइँखोला, सुकेखोला र मन्मत्ता खोला दायाँ बायाँ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">गोरेटो बाटो भएकोमा </t>
+  </si>
+  <si>
+    <t xml:space="preserve">प्लानिंग सम्बन्धी मापदण्ड </t>
+  </si>
+  <si>
+    <t xml:space="preserve">खुलालटार सानागाउँ सडक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">खुलालटार परोपकार बाटो </t>
+  </si>
+  <si>
+    <t xml:space="preserve">खुलालटार सेतिदेवी संकल्प नेपाल बाटो </t>
+  </si>
+  <si>
+    <t xml:space="preserve">खुलालटार माझगाउँ सडक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">खुलालटार गोठगाउँ हुँदै मनमत्ता खोला पुखुलाछी सम्म </t>
+  </si>
+  <si>
+    <t xml:space="preserve">खुलालटार थापागाउँ बानिया टोल सडक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">खुलालटार बेनडोल सडक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">खुलालटार गोठगाउँ इन्द्रायणी बन किनार सडक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">इन्द्रायणी चाँगु सडक </t>
+  </si>
+  <si>
+    <t>खुलालटार सनोकुर्थली माझ गाउँ सडक (४ नं. )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">इन्द्रायणी झो. पु. कृषि सडक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">कुसुम थालि परियार टोल सडक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">इन्द्रायणी मनहरा दोभान सडक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">दिवाकर घर छ्याकापाखा सडक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">रा. उ. मा. वि. छ्याकापाखा सडक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">रा. उ. मा. वि. बानिया गाउँ मनमत्ता सडक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">कुर्थली चोक बाट झोलुङ्गेपुल जाने बाटो </t>
+  </si>
+  <si>
+    <t xml:space="preserve">खुलालटार राजकुलो भित्रि बाटो (भगवान घर) पछाडी </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-4000439]0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,6 +609,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -385,7 +670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -412,6 +697,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,14 +1016,14 @@
       <selection sqref="A1:C58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="68.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -740,7 +1034,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -751,7 +1045,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -762,7 +1056,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -773,7 +1067,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -784,7 +1078,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -795,7 +1089,7 @@
         <v>350000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -806,7 +1100,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -817,7 +1111,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -828,7 +1122,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -839,7 +1133,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>10</v>
       </c>
@@ -850,7 +1144,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>11</v>
       </c>
@@ -861,7 +1155,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>12</v>
       </c>
@@ -872,7 +1166,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -883,7 +1177,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>14</v>
       </c>
@@ -894,7 +1188,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
         <v>15</v>
       </c>
@@ -905,7 +1199,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
         <v>16</v>
       </c>
@@ -916,7 +1210,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
         <v>17</v>
       </c>
@@ -927,7 +1221,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="11">
         <v>18</v>
       </c>
@@ -938,7 +1232,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="11">
         <v>19</v>
       </c>
@@ -949,7 +1243,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -964,13 +1258,13 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="1"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>0</v>
       </c>
@@ -982,13 +1276,13 @@
       </c>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="11">
         <v>21</v>
       </c>
@@ -999,7 +1293,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="11">
         <v>22</v>
       </c>
@@ -1010,7 +1304,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
         <v>23</v>
       </c>
@@ -1021,7 +1315,7 @@
         <v>1600000</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="11">
         <v>24</v>
       </c>
@@ -1032,7 +1326,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="11">
         <v>25</v>
       </c>
@@ -1043,7 +1337,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="11">
         <v>26</v>
       </c>
@@ -1054,21 +1348,21 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="11">
         <v>27</v>
       </c>
@@ -1079,7 +1373,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="11">
         <v>28</v>
       </c>
@@ -1090,14 +1384,14 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="11">
         <v>29</v>
       </c>
@@ -1108,21 +1402,21 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="11">
         <v>30</v>
       </c>
@@ -1133,7 +1427,7 @@
         <v>1600000</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="11">
         <v>31</v>
       </c>
@@ -1144,7 +1438,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="11">
         <v>32</v>
       </c>
@@ -1155,7 +1449,7 @@
         <v>1600000</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="11">
         <v>33</v>
       </c>
@@ -1166,7 +1460,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="11">
         <v>34</v>
       </c>
@@ -1177,7 +1471,7 @@
         <v>2500000</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="15">
         <v>35</v>
       </c>
@@ -1188,13 +1482,13 @@
         <v>2100000</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="11">
         <v>36</v>
       </c>
@@ -1205,13 +1499,13 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="11">
         <v>37</v>
       </c>
@@ -1222,7 +1516,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="11">
         <v>38</v>
       </c>
@@ -1237,20 +1531,20 @@
         <v>19100000</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B50" s="6"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B51" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B52" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>39</v>
       </c>
@@ -1261,12 +1555,12 @@
         <v>1304700</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B55" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>40</v>
       </c>
@@ -1277,13 +1571,13 @@
         <v>2660000</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B57" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>41</v>
       </c>
@@ -1294,7 +1588,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C60" s="9">
         <f>SUM(C2:C58)</f>
         <v>40164700</v>
@@ -1310,26 +1604,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="H8:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="D5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G7" sqref="G7:M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H8" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H9" s="19" t="s">
         <v>58</v>
       </c>
@@ -1346,7 +1640,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H10" s="19">
         <v>1</v>
       </c>
@@ -1361,7 +1655,7 @@
       </c>
       <c r="L10" s="18"/>
     </row>
-    <row r="11" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H11" s="19">
         <v>2</v>
       </c>
@@ -1377,7 +1671,7 @@
       </c>
       <c r="L11" s="18"/>
     </row>
-    <row r="12" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H12" s="19">
         <v>3</v>
       </c>
@@ -1393,7 +1687,7 @@
       </c>
       <c r="L12" s="18"/>
     </row>
-    <row r="13" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H13" s="19">
         <v>4</v>
       </c>
@@ -1408,7 +1702,7 @@
       </c>
       <c r="L13" s="18"/>
     </row>
-    <row r="14" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H14" s="19">
         <v>5</v>
       </c>
@@ -1423,7 +1717,7 @@
       </c>
       <c r="L14" s="18"/>
     </row>
-    <row r="15" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H15" s="19">
         <v>6</v>
       </c>
@@ -1438,7 +1732,7 @@
       </c>
       <c r="L15" s="18"/>
     </row>
-    <row r="16" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H16" s="19">
         <v>7</v>
       </c>
@@ -1453,7 +1747,7 @@
       </c>
       <c r="L16" s="18"/>
     </row>
-    <row r="17" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H17" s="19">
         <v>8</v>
       </c>
@@ -1468,7 +1762,7 @@
       </c>
       <c r="L17" s="18"/>
     </row>
-    <row r="18" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H18" s="19">
         <v>9</v>
       </c>
@@ -1483,7 +1777,7 @@
       </c>
       <c r="L18" s="18"/>
     </row>
-    <row r="19" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H19" s="20">
         <v>10</v>
       </c>
@@ -1507,4 +1801,390 @@
 Er. Prakash Singh Saud</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="49.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="1">
+        <v>220</v>
+      </c>
+      <c r="D6" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="1">
+        <v>800</v>
+      </c>
+      <c r="D10" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="1">
+        <v>350</v>
+      </c>
+      <c r="D11" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="1">
+        <v>850</v>
+      </c>
+      <c r="D12" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="1">
+        <v>80</v>
+      </c>
+      <c r="D17" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B23" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="24">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="1">
+        <v>900</v>
+      </c>
+      <c r="D27" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>116</v>
+      </c>
+      <c r="D35" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>117</v>
+      </c>
+      <c r="D36" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>118</v>
+      </c>
+      <c r="D37" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>119</v>
+      </c>
+      <c r="D38" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>120</v>
+      </c>
+      <c r="D39" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>121</v>
+      </c>
+      <c r="D40" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>122</v>
+      </c>
+      <c r="D41" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>124</v>
+      </c>
+      <c r="D43" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>125</v>
+      </c>
+      <c r="D44" s="1">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
hem/binod khatri tahara printed and sadak estimate for length breadth done with sumitraa dd
</commit_message>
<xml_diff>
--- a/ofc/2081_82 yojana haru.xlsx
+++ b/ofc/2081_82 yojana haru.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$58</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$G$7:$M$20</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -25,6 +25,182 @@
     <author>Author</author>
   </authors>
   <commentList>
+    <comment ref="C5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+approximate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+approximate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+badri dai ko ghar jane baato</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+badri dai ko ghar jane baato</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+ward 8 no. jane baato</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+approximate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+approximate only and not khuleko full</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+nakhuleko baato</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E20" authorId="0" shapeId="0">
       <text>
         <r>
@@ -142,6 +318,292 @@
           </rPr>
           <t xml:space="preserve">
 नेपाल सरकार को मापदण्ड बमोजिम</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C28" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+approximate upto paropakar bhawan</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C29" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+approximate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C30" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+approximate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C31" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+approximate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C32" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+approx</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C34" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+approx</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C37" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+approx</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C38" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+approx</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C39" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+baato xaina</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C40" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+nakhuleko</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C41" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+approx</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C43" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+approximate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C44" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+nakhuleko</t>
         </r>
       </text>
     </comment>
@@ -150,7 +612,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="127">
   <si>
     <t>क्र. सं</t>
   </si>
@@ -545,15 +1007,18 @@
   <si>
     <t xml:space="preserve">खुलालटार राजकुलो भित्रि बाटो (भगवान घर) पछाडी </t>
   </si>
+  <si>
+    <t xml:space="preserve">नखुलेको </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-4000439]0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -621,6 +1086,17 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1016,14 +1492,14 @@
       <selection sqref="A1:C58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="68.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1034,7 +1510,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1045,7 +1521,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1056,7 +1532,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1067,7 +1543,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1078,7 +1554,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1089,7 +1565,7 @@
         <v>350000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -1100,7 +1576,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1111,7 +1587,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -1122,7 +1598,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -1133,7 +1609,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>10</v>
       </c>
@@ -1144,7 +1620,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>11</v>
       </c>
@@ -1155,7 +1631,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>12</v>
       </c>
@@ -1166,7 +1642,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -1177,7 +1653,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>14</v>
       </c>
@@ -1188,7 +1664,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>15</v>
       </c>
@@ -1199,7 +1675,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>16</v>
       </c>
@@ -1210,7 +1686,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>17</v>
       </c>
@@ -1221,7 +1697,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>18</v>
       </c>
@@ -1232,7 +1708,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>19</v>
       </c>
@@ -1243,7 +1719,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1258,13 +1734,13 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="1"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>0</v>
       </c>
@@ -1276,13 +1752,13 @@
       </c>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>21</v>
       </c>
@@ -1293,7 +1769,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>22</v>
       </c>
@@ -1304,7 +1780,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>23</v>
       </c>
@@ -1315,7 +1791,7 @@
         <v>1600000</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>24</v>
       </c>
@@ -1326,7 +1802,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>25</v>
       </c>
@@ -1337,7 +1813,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>26</v>
       </c>
@@ -1348,21 +1824,21 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>27</v>
       </c>
@@ -1373,7 +1849,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>28</v>
       </c>
@@ -1384,14 +1860,14 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
         <v>29</v>
       </c>
@@ -1402,21 +1878,21 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="11">
         <v>30</v>
       </c>
@@ -1427,7 +1903,7 @@
         <v>1600000</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="11">
         <v>31</v>
       </c>
@@ -1438,7 +1914,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
         <v>32</v>
       </c>
@@ -1449,7 +1925,7 @@
         <v>1600000</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="11">
         <v>33</v>
       </c>
@@ -1460,7 +1936,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
         <v>34</v>
       </c>
@@ -1471,7 +1947,7 @@
         <v>2500000</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <v>35</v>
       </c>
@@ -1482,13 +1958,13 @@
         <v>2100000</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
         <v>36</v>
       </c>
@@ -1499,13 +1975,13 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
         <v>37</v>
       </c>
@@ -1516,7 +1992,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="11">
         <v>38</v>
       </c>
@@ -1531,20 +2007,20 @@
         <v>19100000</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>39</v>
       </c>
@@ -1555,12 +2031,12 @@
         <v>1304700</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>40</v>
       </c>
@@ -1571,13 +2047,13 @@
         <v>2660000</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>41</v>
       </c>
@@ -1588,7 +2064,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C60" s="9">
         <f>SUM(C2:C58)</f>
         <v>40164700</v>
@@ -1608,22 +2084,22 @@
       <selection activeCell="G7" sqref="G7:M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" customWidth="1"/>
-    <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H8" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H9" s="19" t="s">
         <v>58</v>
       </c>
@@ -1640,7 +2116,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H10" s="19">
         <v>1</v>
       </c>
@@ -1655,7 +2131,7 @@
       </c>
       <c r="L10" s="18"/>
     </row>
-    <row r="11" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H11" s="19">
         <v>2</v>
       </c>
@@ -1671,7 +2147,7 @@
       </c>
       <c r="L11" s="18"/>
     </row>
-    <row r="12" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H12" s="19">
         <v>3</v>
       </c>
@@ -1687,7 +2163,7 @@
       </c>
       <c r="L12" s="18"/>
     </row>
-    <row r="13" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H13" s="19">
         <v>4</v>
       </c>
@@ -1702,7 +2178,7 @@
       </c>
       <c r="L13" s="18"/>
     </row>
-    <row r="14" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H14" s="19">
         <v>5</v>
       </c>
@@ -1717,7 +2193,7 @@
       </c>
       <c r="L14" s="18"/>
     </row>
-    <row r="15" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H15" s="19">
         <v>6</v>
       </c>
@@ -1732,7 +2208,7 @@
       </c>
       <c r="L15" s="18"/>
     </row>
-    <row r="16" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H16" s="19">
         <v>7</v>
       </c>
@@ -1747,7 +2223,7 @@
       </c>
       <c r="L16" s="18"/>
     </row>
-    <row r="17" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H17" s="19">
         <v>8</v>
       </c>
@@ -1762,7 +2238,7 @@
       </c>
       <c r="L17" s="18"/>
     </row>
-    <row r="18" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H18" s="19">
         <v>9</v>
       </c>
@@ -1777,7 +2253,7 @@
       </c>
       <c r="L18" s="18"/>
     </row>
-    <row r="19" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H19" s="20">
         <v>10</v>
       </c>
@@ -1807,16 +2283,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>79</v>
       </c>
@@ -1833,7 +2309,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>84</v>
       </c>
@@ -1844,7 +2320,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>85</v>
       </c>
@@ -1855,26 +2331,26 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>87</v>
       </c>
-      <c r="C4" t="s">
-        <v>86</v>
-      </c>
       <c r="D4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>88</v>
       </c>
+      <c r="C5" s="1">
+        <v>500</v>
+      </c>
       <c r="D5" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>89</v>
       </c>
@@ -1885,31 +2361,40 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>90</v>
       </c>
+      <c r="C7">
+        <v>130</v>
+      </c>
       <c r="D7" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>100</v>
       </c>
       <c r="D8" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>91</v>
       </c>
       <c r="D9" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>92</v>
       </c>
@@ -1920,7 +2405,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>93</v>
       </c>
@@ -1931,7 +2416,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>94</v>
       </c>
@@ -1942,31 +2427,40 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>95</v>
       </c>
+      <c r="C13" s="1">
+        <v>260</v>
+      </c>
       <c r="D13" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>96</v>
       </c>
+      <c r="C14" s="1">
+        <v>350</v>
+      </c>
       <c r="D14" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>97</v>
       </c>
+      <c r="C15" s="1">
+        <v>120</v>
+      </c>
       <c r="D15" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>98</v>
       </c>
@@ -1974,18 +2468,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+    <row r="17" spans="2:5" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="24">
         <v>80</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="24">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>101</v>
       </c>
@@ -1993,7 +2487,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>102</v>
       </c>
@@ -2001,7 +2495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>103</v>
       </c>
@@ -2009,12 +2503,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="2:5" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="22" t="s">
         <v>105</v>
       </c>
@@ -2022,7 +2516,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>106</v>
       </c>
@@ -2030,12 +2524,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>108</v>
       </c>
@@ -2046,95 +2540,129 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>109</v>
       </c>
+      <c r="C28">
+        <v>53</v>
+      </c>
       <c r="D28" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>110</v>
       </c>
+      <c r="C29">
+        <f>390+200</f>
+        <v>590</v>
+      </c>
       <c r="D29" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>111</v>
       </c>
+      <c r="C30">
+        <v>230</v>
+      </c>
       <c r="D30" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>112</v>
       </c>
+      <c r="C31">
+        <v>650</v>
+      </c>
       <c r="D31" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>113</v>
       </c>
+      <c r="C32">
+        <v>460</v>
+      </c>
       <c r="D32" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>114</v>
       </c>
+      <c r="C33" s="1">
+        <v>800</v>
+      </c>
       <c r="D33" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>115</v>
       </c>
+      <c r="C34">
+        <v>330</v>
+      </c>
       <c r="D34" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>116</v>
       </c>
+      <c r="C35" s="1">
+        <v>600</v>
+      </c>
       <c r="D35" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>117</v>
       </c>
+      <c r="C36">
+        <v>210</v>
+      </c>
       <c r="D36" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>118</v>
       </c>
+      <c r="C37" s="1">
+        <v>250</v>
+      </c>
       <c r="D37" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>119</v>
       </c>
+      <c r="C38">
+        <v>130</v>
+      </c>
       <c r="D38" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>120</v>
       </c>
@@ -2142,7 +2670,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>121</v>
       </c>
@@ -2150,31 +2678,40 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>122</v>
       </c>
+      <c r="C41">
+        <v>100</v>
+      </c>
       <c r="D41" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>123</v>
       </c>
+      <c r="C42">
+        <v>464</v>
+      </c>
       <c r="D42" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>124</v>
       </c>
+      <c r="C43">
+        <v>370</v>
+      </c>
       <c r="D43" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>125</v>
       </c>

</xml_diff>

<commit_message>
continue of kalika mandir sauchalaya and bibaran to nova mam
</commit_message>
<xml_diff>
--- a/ofc/2081_82 yojana haru.xlsx
+++ b/ofc/2081_82 yojana haru.xlsx
@@ -4,15 +4,17 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Baato" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1 (2)" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$58</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Sheet1 (2)'!$C$5:$D$10</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$G$7:$M$20</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -612,7 +614,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="127">
   <si>
     <t>क्र. सं</t>
   </si>
@@ -1146,7 +1148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1182,6 +1184,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1489,8 +1502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A16" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C58"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2284,8 +2297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2921,4 +2934,75 @@
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:D10"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:4" s="29" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="30">
+        <v>1</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="30">
+        <v>2</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="30">
+        <v>3</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="30">
+        <v>4</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="30">
+        <v>5</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="85" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
bibaran upgraded for prakash sir and kurthali complete
</commit_message>
<xml_diff>
--- a/ofc/2081_82 yojana haru.xlsx
+++ b/ofc/2081_82 yojana haru.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Sheet1 (2)'!$C$5:$D$10</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$G$7:$M$20</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -614,7 +614,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="138">
   <si>
     <t>क्र. सं</t>
   </si>
@@ -1012,11 +1012,44 @@
   <si>
     <t xml:space="preserve">नखुलेको </t>
   </si>
+  <si>
+    <t>KM</t>
+  </si>
+  <si>
+    <t>Gravel road</t>
+  </si>
+  <si>
+    <t>Sauchalaya nirman</t>
+  </si>
+  <si>
+    <t>Pahiro hataune/samrakxan</t>
+  </si>
+  <si>
+    <t>Gabion</t>
+  </si>
+  <si>
+    <t>cum</t>
+  </si>
+  <si>
+    <t>Rubble masonary</t>
+  </si>
+  <si>
+    <t>road upgrading/levelling</t>
+  </si>
+  <si>
+    <t>sqm</t>
+  </si>
+  <si>
+    <t>Plum wall</t>
+  </si>
+  <si>
+    <t>School maintainance</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-4000439]0"/>
   </numFmts>
@@ -1148,7 +1181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1196,6 +1229,20 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1502,18 +1549,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="68.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1524,7 +1571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1535,7 +1582,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1546,7 +1593,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1557,7 +1604,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1568,7 +1615,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1579,7 +1626,7 @@
         <v>350000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -1590,7 +1637,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1601,7 +1648,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -1612,7 +1659,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -1623,7 +1670,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>10</v>
       </c>
@@ -1634,7 +1681,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>11</v>
       </c>
@@ -1645,7 +1692,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>12</v>
       </c>
@@ -1656,7 +1703,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -1667,7 +1714,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>14</v>
       </c>
@@ -1678,7 +1725,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
         <v>15</v>
       </c>
@@ -1689,7 +1736,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
         <v>16</v>
       </c>
@@ -1700,7 +1747,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
         <v>17</v>
       </c>
@@ -1711,7 +1758,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="11">
         <v>18</v>
       </c>
@@ -1722,7 +1769,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="11">
         <v>19</v>
       </c>
@@ -1733,7 +1780,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1748,13 +1795,13 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="1"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>0</v>
       </c>
@@ -1766,13 +1813,13 @@
       </c>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="11">
         <v>21</v>
       </c>
@@ -1783,7 +1830,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="11">
         <v>22</v>
       </c>
@@ -1794,7 +1841,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
         <v>23</v>
       </c>
@@ -1805,7 +1852,7 @@
         <v>1600000</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="11">
         <v>24</v>
       </c>
@@ -1816,7 +1863,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="11">
         <v>25</v>
       </c>
@@ -1827,7 +1874,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="11">
         <v>26</v>
       </c>
@@ -1838,21 +1885,21 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="11">
         <v>27</v>
       </c>
@@ -1863,7 +1910,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="11">
         <v>28</v>
       </c>
@@ -1874,14 +1921,14 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="11">
         <v>29</v>
       </c>
@@ -1892,21 +1939,21 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="11">
         <v>30</v>
       </c>
@@ -1917,7 +1964,7 @@
         <v>1600000</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="11">
         <v>31</v>
       </c>
@@ -1928,7 +1975,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="11">
         <v>32</v>
       </c>
@@ -1939,7 +1986,7 @@
         <v>1600000</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="11">
         <v>33</v>
       </c>
@@ -1950,7 +1997,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="11">
         <v>34</v>
       </c>
@@ -1961,7 +2008,7 @@
         <v>2500000</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="15">
         <v>35</v>
       </c>
@@ -1972,13 +2019,13 @@
         <v>2100000</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="11">
         <v>36</v>
       </c>
@@ -1989,13 +2036,13 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="11">
         <v>37</v>
       </c>
@@ -2006,7 +2053,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="11">
         <v>38</v>
       </c>
@@ -2021,20 +2068,20 @@
         <v>19100000</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B50" s="6"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B51" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B52" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>39</v>
       </c>
@@ -2045,12 +2092,12 @@
         <v>1304700</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B55" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>40</v>
       </c>
@@ -2061,13 +2108,13 @@
         <v>2660000</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B57" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>41</v>
       </c>
@@ -2078,7 +2125,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C60" s="9">
         <f>SUM(C2:C58)</f>
         <v>40164700</v>
@@ -2092,28 +2139,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="H8:L19"/>
+  <dimension ref="H8:L38"/>
   <sheetViews>
-    <sheetView topLeftCell="D5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:M20"/>
+    <sheetView tabSelected="1" topLeftCell="C21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H8" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H9" s="19" t="s">
         <v>58</v>
       </c>
@@ -2130,7 +2177,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H10" s="19">
         <v>1</v>
       </c>
@@ -2145,7 +2192,7 @@
       </c>
       <c r="L10" s="18"/>
     </row>
-    <row r="11" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H11" s="19">
         <v>2</v>
       </c>
@@ -2161,7 +2208,7 @@
       </c>
       <c r="L11" s="18"/>
     </row>
-    <row r="12" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H12" s="19">
         <v>3</v>
       </c>
@@ -2177,7 +2224,7 @@
       </c>
       <c r="L12" s="18"/>
     </row>
-    <row r="13" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H13" s="19">
         <v>4</v>
       </c>
@@ -2192,7 +2239,7 @@
       </c>
       <c r="L13" s="18"/>
     </row>
-    <row r="14" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H14" s="19">
         <v>5</v>
       </c>
@@ -2207,7 +2254,7 @@
       </c>
       <c r="L14" s="18"/>
     </row>
-    <row r="15" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H15" s="19">
         <v>6</v>
       </c>
@@ -2222,7 +2269,7 @@
       </c>
       <c r="L15" s="18"/>
     </row>
-    <row r="16" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H16" s="19">
         <v>7</v>
       </c>
@@ -2237,7 +2284,7 @@
       </c>
       <c r="L16" s="18"/>
     </row>
-    <row r="17" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H17" s="19">
         <v>8</v>
       </c>
@@ -2252,7 +2299,7 @@
       </c>
       <c r="L17" s="18"/>
     </row>
-    <row r="18" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H18" s="19">
         <v>9</v>
       </c>
@@ -2267,7 +2314,7 @@
       </c>
       <c r="L18" s="18"/>
     </row>
-    <row r="19" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:12" x14ac:dyDescent="0.3">
       <c r="H19" s="20">
         <v>10</v>
       </c>
@@ -2281,6 +2328,263 @@
         <v>2</v>
       </c>
       <c r="L19" s="18"/>
+    </row>
+    <row r="22" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H22" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H23" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="I23" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="J23" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="K23" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="L23" s="31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H24" s="32">
+        <v>1</v>
+      </c>
+      <c r="I24" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="J24" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="K24" s="33">
+        <v>4</v>
+      </c>
+      <c r="L24" s="33"/>
+    </row>
+    <row r="25" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H25" s="32">
+        <v>2</v>
+      </c>
+      <c r="I25" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="J25" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="K25" s="33">
+        <f>(87.3+103.72)/1000</f>
+        <v>0.19102</v>
+      </c>
+      <c r="L25" s="33"/>
+    </row>
+    <row r="26" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H26" s="32">
+        <v>3</v>
+      </c>
+      <c r="I26" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="J26" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="K26" s="33">
+        <f>1+1+1+1+1</f>
+        <v>5</v>
+      </c>
+      <c r="L26" s="33"/>
+    </row>
+    <row r="27" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H27" s="32">
+        <v>4</v>
+      </c>
+      <c r="I27" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="J27" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="K27" s="33">
+        <v>1</v>
+      </c>
+      <c r="L27" s="33"/>
+    </row>
+    <row r="28" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H28" s="32">
+        <v>5</v>
+      </c>
+      <c r="I28" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="J28" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="K28" s="33">
+        <f>1+1+1+1+1</f>
+        <v>5</v>
+      </c>
+      <c r="L28" s="33"/>
+    </row>
+    <row r="29" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H29" s="32">
+        <v>6</v>
+      </c>
+      <c r="I29" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="J29" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="K29" s="33">
+        <f>65+10+10+12.5</f>
+        <v>97.5</v>
+      </c>
+      <c r="L29" s="33"/>
+    </row>
+    <row r="30" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H30" s="32">
+        <v>7</v>
+      </c>
+      <c r="I30" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="J30" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="K30" s="34">
+        <v>2</v>
+      </c>
+      <c r="L30" s="33"/>
+    </row>
+    <row r="31" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H31" s="32">
+        <v>8</v>
+      </c>
+      <c r="I31" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="J31" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="K31" s="34">
+        <f>78+3</f>
+        <v>81</v>
+      </c>
+      <c r="L31" s="33"/>
+    </row>
+    <row r="32" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H32" s="32">
+        <v>9</v>
+      </c>
+      <c r="I32" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="J32" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="K32" s="34">
+        <f>13.8+47.18+32.27+13.34+34.56+8.8+30.07+5.3</f>
+        <v>185.32000000000002</v>
+      </c>
+      <c r="L32" s="33"/>
+    </row>
+    <row r="33" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H33" s="32">
+        <v>10</v>
+      </c>
+      <c r="I33" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="J33" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="K33" s="33">
+        <f>(17.2+6.5+13.8+20.2)/1000</f>
+        <v>5.7700000000000001E-2</v>
+      </c>
+      <c r="L33" s="33"/>
+    </row>
+    <row r="34" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H34" s="32">
+        <v>11</v>
+      </c>
+      <c r="I34" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="J34" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="K34" s="33">
+        <f>147/100</f>
+        <v>1.47</v>
+      </c>
+      <c r="L34" s="33"/>
+    </row>
+    <row r="35" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H35" s="32">
+        <v>12</v>
+      </c>
+      <c r="I35" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="J35" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="K35" s="33">
+        <v>1</v>
+      </c>
+      <c r="L35" s="33"/>
+    </row>
+    <row r="36" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H36" s="32">
+        <v>13</v>
+      </c>
+      <c r="I36" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="J36" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="K36" s="33">
+        <f>42.21+11.02</f>
+        <v>53.230000000000004</v>
+      </c>
+      <c r="L36" s="33"/>
+    </row>
+    <row r="37" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H37" s="32">
+        <v>14</v>
+      </c>
+      <c r="I37" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="J37" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="K37" s="33">
+        <f>22.43+44.02</f>
+        <v>66.45</v>
+      </c>
+      <c r="L37" s="33"/>
+    </row>
+    <row r="38" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H38" s="32">
+        <v>15</v>
+      </c>
+      <c r="I38" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="J38" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="K38" s="33">
+        <v>1</v>
+      </c>
+      <c r="L38" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2301,12 +2605,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>79</v>
       </c>
@@ -2323,7 +2627,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="23">
         <v>1</v>
       </c>
@@ -2338,7 +2642,7 @@
       </c>
       <c r="E2" s="18"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="23">
         <v>2</v>
       </c>
@@ -2353,7 +2657,7 @@
       </c>
       <c r="E3" s="18"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="23">
         <v>3</v>
       </c>
@@ -2366,7 +2670,7 @@
       </c>
       <c r="E4" s="18"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="23">
         <v>4</v>
       </c>
@@ -2381,7 +2685,7 @@
       </c>
       <c r="E5" s="18"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="23">
         <v>5</v>
       </c>
@@ -2396,7 +2700,7 @@
       </c>
       <c r="E6" s="18"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="23">
         <v>6</v>
       </c>
@@ -2411,7 +2715,7 @@
       </c>
       <c r="E7" s="18"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="23">
         <v>7</v>
       </c>
@@ -2426,7 +2730,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="23">
         <v>8</v>
       </c>
@@ -2441,7 +2745,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="23">
         <v>9</v>
       </c>
@@ -2456,7 +2760,7 @@
       </c>
       <c r="E10" s="18"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="23">
         <v>10</v>
       </c>
@@ -2471,7 +2775,7 @@
       </c>
       <c r="E11" s="18"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="23">
         <v>11</v>
       </c>
@@ -2487,7 +2791,7 @@
       <c r="E12" s="18"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="23">
         <v>12</v>
       </c>
@@ -2502,7 +2806,7 @@
       </c>
       <c r="E13" s="18"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="23">
         <v>13</v>
       </c>
@@ -2517,7 +2821,7 @@
       </c>
       <c r="E14" s="18"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="23">
         <v>14</v>
       </c>
@@ -2532,7 +2836,7 @@
       </c>
       <c r="E15" s="18"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="23">
         <v>15</v>
       </c>
@@ -2545,7 +2849,7 @@
       </c>
       <c r="E16" s="18"/>
     </row>
-    <row r="17" spans="1:5" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="23">
         <v>16</v>
       </c>
@@ -2560,14 +2864,14 @@
       </c>
       <c r="E17" s="25"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="18"/>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
       <c r="E18" s="18"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="23">
         <v>17</v>
       </c>
@@ -2582,7 +2886,7 @@
       </c>
       <c r="E19" s="18"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="23">
         <v>17.714285714285701</v>
       </c>
@@ -2597,7 +2901,7 @@
       </c>
       <c r="E20" s="18"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="23">
         <v>18.428571428571399</v>
       </c>
@@ -2613,7 +2917,7 @@
       </c>
       <c r="E21" s="18"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="23">
         <v>19.1428571428571</v>
       </c>
@@ -2628,7 +2932,7 @@
       </c>
       <c r="E22" s="18"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="23">
         <v>19.857142857142801</v>
       </c>
@@ -2643,7 +2947,7 @@
       </c>
       <c r="E23" s="18"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="23">
         <v>20.571428571428498</v>
       </c>
@@ -2658,7 +2962,7 @@
       </c>
       <c r="E24" s="18"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="23">
         <v>21.285714285714199</v>
       </c>
@@ -2673,7 +2977,7 @@
       </c>
       <c r="E25" s="18"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="23">
         <v>21.999999999999901</v>
       </c>
@@ -2688,7 +2992,7 @@
       </c>
       <c r="E26" s="18"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="23">
         <v>22.714285714285602</v>
       </c>
@@ -2703,7 +3007,7 @@
       </c>
       <c r="E27" s="18"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="23">
         <v>23.428571428571299</v>
       </c>
@@ -2718,7 +3022,7 @@
       </c>
       <c r="E28" s="18"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="23">
         <v>24.142857142857</v>
       </c>
@@ -2733,7 +3037,7 @@
       </c>
       <c r="E29" s="18"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="23">
         <v>24.857142857142701</v>
       </c>
@@ -2748,7 +3052,7 @@
       </c>
       <c r="E30" s="18"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="23">
         <v>25.571428571428399</v>
       </c>
@@ -2761,7 +3065,7 @@
       </c>
       <c r="E31" s="18"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="23">
         <v>26.2857142857141</v>
       </c>
@@ -2774,7 +3078,7 @@
       </c>
       <c r="E32" s="18"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="23">
         <v>26.999999999999801</v>
       </c>
@@ -2789,7 +3093,7 @@
       </c>
       <c r="E33" s="18"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="23">
         <v>27.714285714285499</v>
       </c>
@@ -2804,7 +3108,7 @@
       </c>
       <c r="E34" s="18"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="23">
         <v>28.4285714285712</v>
       </c>
@@ -2819,7 +3123,7 @@
       </c>
       <c r="E35" s="18"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="23">
         <v>29.142857142856901</v>
       </c>
@@ -2832,14 +3136,14 @@
       </c>
       <c r="E36" s="18"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="18"/>
       <c r="B37" s="18"/>
       <c r="C37" s="23"/>
       <c r="D37" s="23"/>
       <c r="E37" s="18"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="23">
         <v>1</v>
       </c>
@@ -2852,7 +3156,7 @@
       </c>
       <c r="E38" s="18"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="23">
         <v>2</v>
       </c>
@@ -2865,7 +3169,7 @@
       </c>
       <c r="E39" s="18"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="23">
         <v>3</v>
       </c>
@@ -2878,7 +3182,7 @@
       </c>
       <c r="E40" s="18"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="23">
         <v>4</v>
       </c>
@@ -2889,7 +3193,7 @@
       <c r="D41" s="23"/>
       <c r="E41" s="18"/>
     </row>
-    <row r="42" spans="1:5" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" s="22" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="23">
         <v>5</v>
       </c>
@@ -2902,7 +3206,7 @@
       </c>
       <c r="E42" s="25"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="23">
         <v>6</v>
       </c>
@@ -2915,7 +3219,7 @@
       </c>
       <c r="E43" s="18"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="23">
         <v>7</v>
       </c>
@@ -2926,7 +3230,7 @@
       <c r="D44" s="23"/>
       <c r="E44" s="18"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
     </row>
   </sheetData>
@@ -2944,16 +3248,16 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:4" s="29" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:4" s="29" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C5" s="28" t="s">
         <v>0</v>
       </c>
@@ -2961,7 +3265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C6" s="30">
         <v>1</v>
       </c>
@@ -2969,7 +3273,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C7" s="30">
         <v>2</v>
       </c>
@@ -2977,7 +3281,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C8" s="30">
         <v>3</v>
       </c>
@@ -2985,7 +3289,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C9" s="30">
         <v>4</v>
       </c>
@@ -2993,7 +3297,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C10" s="30">
         <v>5</v>
       </c>

</xml_diff>